<commit_message>
2nd term results added
</commit_message>
<xml_diff>
--- a/test_results.xlsx
+++ b/test_results.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olczy/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olczy/Desktop/materiały/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BD4713-CB61-0541-BCE3-8E21C9FAA721}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3529ED36-5344-AC47-B085-932060DC8AE3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9800" yWindow="5240" windowWidth="28040" windowHeight="16100" xr2:uid="{F45F0B64-4A9A-0347-9C61-90EE7F6B8E00}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" activeTab="1" xr2:uid="{F45F0B64-4A9A-0347-9C61-90EE7F6B8E00}"/>
   </bookViews>
   <sheets>
-    <sheet name="test" sheetId="2" r:id="rId1"/>
+    <sheet name="test 1st term" sheetId="2" r:id="rId1"/>
+    <sheet name="test 2nd term" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -583,73 +584,239 @@
         </r>
       </text>
     </comment>
-    <comment ref="C15" authorId="0" shapeId="0" xr:uid="{BE7133B9-582C-FF41-8B07-3BEBC2CF1D82}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t>writing on 4th April</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C16" authorId="0" shapeId="0" xr:uid="{EBAA0DCB-5E3F-9E43-B665-DCAE03E97E97}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t>writing on 4th April</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C17" authorId="0" shapeId="0" xr:uid="{C36D6BB4-3D95-6341-9236-17EFDF50E88C}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t>writing on 4th April</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C18" authorId="0" shapeId="0" xr:uid="{AAB3F8B1-82AA-B14C-9E16-E4F3D54AC85A}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t>writing on 4th April</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C19" authorId="0" shapeId="0" xr:uid="{3A9E6DD4-559B-FC45-AD0C-A26EB8247457}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t>???</t>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Aleksander Krzysztof NOSARZEWSKI</author>
+  </authors>
+  <commentList>
+    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{73EA90F4-00B5-D84E-BCA1-925158BF221D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">no answer
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T3" authorId="0" shapeId="0" xr:uid="{B93278A3-736D-654E-BEE6-7FFF7993CE4F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">no FPR
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{1F7A888B-AD60-7045-97D6-76035BEA4FFA}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>no seed set</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{D39A23E5-D331-444A-875E-6660D9E8131E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>should be 10 trees, not 100</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{06D15B5D-0057-914F-B243-2A8158CC6E2D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>for making predictions on validation set</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K4" authorId="0" shapeId="0" xr:uid="{8C363174-FFCB-784F-B1F5-FA450FE6B1D9}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>NAs, not NaNs ;)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M4" authorId="0" shapeId="0" xr:uid="{D99EB5E9-27BC-4D44-87DA-DA8E78B1EF31}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>using barplot would give MUCH tidier result</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N4" authorId="0" shapeId="0" xr:uid="{B6CE0B2A-D7EF-574B-AD1C-B50A6DE6B924}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>correct but there are easier ways of doing it requiring only one line of code ;)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q4" authorId="0" shapeId="0" xr:uid="{EB474620-C7C4-B34D-ACDC-77B0B1D07115}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>you have chosen cp based on dataset containing row names as variable, but logic is clear and correct</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{6B32A9BA-E01D-3345-BE1A-BC7BA1C57C0E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">aim was to fit linear regression, to binary one </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{A4DC8417-CD85-C644-A983-30DC6589B1F9}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">aim was to fit linear regression, to binary one </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M5" authorId="0" shapeId="0" xr:uid="{01A198A2-CA89-4343-AEF0-06C09AAB8EE9}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>using barplot would give MUCH tidier result</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q5" authorId="0" shapeId="0" xr:uid="{788D3F9C-0098-C848-B1F0-D448FAF5B470}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>no answer</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I6" authorId="0" shapeId="0" xr:uid="{D6A569FC-FE2C-0541-8178-3E93683F3DDD}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>it is actually second model, you calculated everything correctly but 5,06 is smaller than 5,07</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M6" authorId="0" shapeId="0" xr:uid="{5F85BA0C-6DFA-B24E-9625-56EF25A183EB}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>using barplot would give tidier result</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{C15B4C07-D8E0-E04B-96B8-24FDC1835E30}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>not present on any test</t>
         </r>
       </text>
     </comment>
@@ -658,7 +825,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
   <si>
     <t>Student ID</t>
   </si>
@@ -736,6 +903,27 @@
   </si>
   <si>
     <t>Min. exam pts to pass course</t>
+  </si>
+  <si>
+    <t>Ex 1 (12p)</t>
+  </si>
+  <si>
+    <t>Total (13p)</t>
+  </si>
+  <si>
+    <t>4 (3p)</t>
+  </si>
+  <si>
+    <t>5 (2p)</t>
+  </si>
+  <si>
+    <t>6 (3p)</t>
+  </si>
+  <si>
+    <t>11 (1p)</t>
+  </si>
+  <si>
+    <t>12 (2p)</t>
   </si>
 </sst>
 </file>
@@ -818,7 +1006,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -840,13 +1028,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Dziesiętny" xfId="1" builtinId="3"/>
@@ -1163,13 +1355,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FF1BE30-0C18-6D48-B528-712D4FF4354F}">
-  <dimension ref="A1:AA19"/>
+  <dimension ref="A1:AA14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Y21" sqref="Y21"/>
+      <selection pane="bottomRight" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -1177,61 +1369,61 @@
     <col min="1" max="1" width="10.83203125" style="5"/>
     <col min="4" max="9" width="10.83203125" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="10" max="10" width="10.83203125" collapsed="1"/>
-    <col min="11" max="22" width="0" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="22" width="10.83203125" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="23" max="23" width="10.83203125" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="10" t="s">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10" t="s">
+      <c r="D1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10" t="s">
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="10" t="s">
+      <c r="Y1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="10" t="s">
+      <c r="Z1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="11" t="s">
+      <c r="AA1" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
       <c r="D2" s="7" t="s">
         <v>3</v>
       </c>
@@ -1292,10 +1484,10 @@
       <c r="W2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="10"/>
-      <c r="AA2" s="11"/>
+      <c r="X2" s="13"/>
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="13"/>
+      <c r="AA2" s="14"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" s="9">
@@ -1373,11 +1565,11 @@
         <f t="shared" ref="X3:X13" si="2">SUM(C3,J3,W3)</f>
         <v>46.5</v>
       </c>
-      <c r="Y3" s="12">
+      <c r="Y3" s="11">
         <f t="shared" ref="Y3:Y13" si="3">MIN(B3+X3,50)</f>
         <v>46.5</v>
       </c>
-      <c r="Z3" s="13">
+      <c r="Z3" s="12">
         <f t="shared" ref="Z3:Z13" si="4">Y3/50</f>
         <v>0.93</v>
       </c>
@@ -1462,11 +1654,11 @@
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
-      <c r="Y4" s="12">
+      <c r="Y4" s="11">
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="Z4" s="13">
+      <c r="Z4" s="12">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -1551,11 +1743,11 @@
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="Y5" s="12">
+      <c r="Y5" s="11">
         <f t="shared" si="3"/>
         <v>34</v>
       </c>
-      <c r="Z5" s="13">
+      <c r="Z5" s="12">
         <f t="shared" si="4"/>
         <v>0.68</v>
       </c>
@@ -1640,11 +1832,11 @@
         <f t="shared" si="2"/>
         <v>24.5</v>
       </c>
-      <c r="Y6" s="12">
+      <c r="Y6" s="11">
         <f t="shared" si="3"/>
         <v>24.5</v>
       </c>
-      <c r="Z6" s="13">
+      <c r="Z6" s="12">
         <f t="shared" si="4"/>
         <v>0.49</v>
       </c>
@@ -1729,11 +1921,11 @@
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="Y7" s="12">
+      <c r="Y7" s="11">
         <f t="shared" si="3"/>
         <v>36</v>
       </c>
-      <c r="Z7" s="13">
+      <c r="Z7" s="12">
         <f t="shared" si="4"/>
         <v>0.72</v>
       </c>
@@ -1818,11 +2010,11 @@
         <f t="shared" si="2"/>
         <v>41.5</v>
       </c>
-      <c r="Y8" s="12">
+      <c r="Y8" s="11">
         <f t="shared" si="3"/>
         <v>42.5</v>
       </c>
-      <c r="Z8" s="13">
+      <c r="Z8" s="12">
         <f t="shared" si="4"/>
         <v>0.85</v>
       </c>
@@ -1907,11 +2099,11 @@
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
-      <c r="Y9" s="12">
+      <c r="Y9" s="11">
         <f t="shared" si="3"/>
         <v>47</v>
       </c>
-      <c r="Z9" s="13">
+      <c r="Z9" s="12">
         <f t="shared" si="4"/>
         <v>0.94</v>
       </c>
@@ -1996,11 +2188,11 @@
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="Y10" s="12">
+      <c r="Y10" s="11">
         <f t="shared" si="3"/>
         <v>31</v>
       </c>
-      <c r="Z10" s="13">
+      <c r="Z10" s="12">
         <f t="shared" si="4"/>
         <v>0.62</v>
       </c>
@@ -2085,11 +2277,11 @@
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="Y11" s="12">
+      <c r="Y11" s="11">
         <f t="shared" si="3"/>
         <v>39</v>
       </c>
-      <c r="Z11" s="13">
+      <c r="Z11" s="12">
         <f t="shared" si="4"/>
         <v>0.78</v>
       </c>
@@ -2174,11 +2366,11 @@
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="Y12" s="12">
+      <c r="Y12" s="11">
         <f t="shared" si="3"/>
         <v>45</v>
       </c>
-      <c r="Z12" s="13">
+      <c r="Z12" s="12">
         <f t="shared" si="4"/>
         <v>0.9</v>
       </c>
@@ -2263,11 +2455,11 @@
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="Y13" s="12">
+      <c r="Y13" s="11">
         <f t="shared" si="3"/>
         <v>35</v>
       </c>
-      <c r="Z13" s="13">
+      <c r="Z13" s="12">
         <f t="shared" si="4"/>
         <v>0.7</v>
       </c>
@@ -2305,77 +2497,8 @@
       <c r="Z14" s="4"/>
       <c r="AA14" s="3"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A15" s="9">
-        <v>53474</v>
-      </c>
-      <c r="B15" s="1">
-        <v>5</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="2"/>
-      <c r="U15" s="2"/>
-      <c r="V15" s="2"/>
-      <c r="W15" s="2"/>
-      <c r="X15" s="2"/>
-      <c r="Y15" s="3"/>
-      <c r="Z15" s="4"/>
-      <c r="AA15" s="3"/>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A16" s="9">
-        <v>56280</v>
-      </c>
-      <c r="B16" s="1">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="9">
-        <v>74496</v>
-      </c>
-      <c r="B17" s="1">
-        <v>5</v>
-      </c>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="9">
-        <v>63991</v>
-      </c>
-      <c r="B18" s="1">
-        <v>3</v>
-      </c>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="9">
-        <v>79014</v>
-      </c>
-      <c r="B19" s="1">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="D1:J1"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
@@ -2384,6 +2507,568 @@
     <mergeCell ref="Y1:Y2"/>
     <mergeCell ref="Z1:Z2"/>
     <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="D1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A6D02D5-CEF6-ED41-A4EB-1FDB5306AC9C}">
+  <dimension ref="A1:AA7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="Z17" sqref="Z17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="5"/>
+    <col min="4" max="9" width="10.83203125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="10.83203125" collapsed="1"/>
+    <col min="11" max="22" width="10.83203125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="23" max="23" width="10.83203125" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="U2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="V2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="W2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="X2" s="13"/>
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="13"/>
+      <c r="AA2" s="14"/>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A3" s="10">
+        <v>53474</v>
+      </c>
+      <c r="B3" s="1">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2">
+        <v>3</v>
+      </c>
+      <c r="H3" s="2">
+        <v>2</v>
+      </c>
+      <c r="I3" s="2">
+        <v>2</v>
+      </c>
+      <c r="J3" s="2">
+        <f>SUM(D3:I3)</f>
+        <v>12</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1</v>
+      </c>
+      <c r="L3" s="2">
+        <v>2</v>
+      </c>
+      <c r="M3" s="2">
+        <v>2</v>
+      </c>
+      <c r="N3" s="2">
+        <v>2</v>
+      </c>
+      <c r="O3" s="2">
+        <v>1</v>
+      </c>
+      <c r="P3" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>3</v>
+      </c>
+      <c r="R3" s="2">
+        <v>2</v>
+      </c>
+      <c r="S3" s="2">
+        <v>0</v>
+      </c>
+      <c r="T3" s="2">
+        <v>4</v>
+      </c>
+      <c r="U3" s="2">
+        <v>0</v>
+      </c>
+      <c r="V3" s="15">
+        <v>0</v>
+      </c>
+      <c r="W3" s="2">
+        <f>SUM(K3:V3)</f>
+        <v>18</v>
+      </c>
+      <c r="X3" s="2">
+        <f t="shared" ref="X3:X7" si="0">SUM(C3,J3,W3)</f>
+        <v>42</v>
+      </c>
+      <c r="Y3" s="11">
+        <f t="shared" ref="Y3:Y7" si="1">MIN(B3+X3,50)</f>
+        <v>47</v>
+      </c>
+      <c r="Z3" s="12">
+        <f t="shared" ref="Z3:Z7" si="2">Y3/50</f>
+        <v>0.94</v>
+      </c>
+      <c r="AA3" s="3">
+        <f t="shared" ref="AA3:AA7" si="3">50-Y3</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A4" s="10">
+        <v>56280</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2">
+        <v>3</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2">
+        <f>SUM(D4:I4)</f>
+        <v>9</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1</v>
+      </c>
+      <c r="L4" s="2">
+        <v>2</v>
+      </c>
+      <c r="M4" s="2">
+        <v>1</v>
+      </c>
+      <c r="N4" s="2">
+        <v>2</v>
+      </c>
+      <c r="O4" s="2">
+        <v>1</v>
+      </c>
+      <c r="P4" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>2</v>
+      </c>
+      <c r="R4" s="2">
+        <v>2</v>
+      </c>
+      <c r="S4" s="2">
+        <v>0</v>
+      </c>
+      <c r="T4" s="2">
+        <v>1</v>
+      </c>
+      <c r="U4" s="2">
+        <v>0</v>
+      </c>
+      <c r="V4" s="2">
+        <v>0</v>
+      </c>
+      <c r="W4" s="2">
+        <f>SUM(K4:V4)</f>
+        <v>13</v>
+      </c>
+      <c r="X4" s="2">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="Y4" s="11">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="Z4" s="12">
+        <f t="shared" si="2"/>
+        <v>0.7</v>
+      </c>
+      <c r="AA4" s="3">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A5" s="10">
+        <v>74496</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <f>SUM(D5:I5)</f>
+        <v>8</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1</v>
+      </c>
+      <c r="L5" s="2">
+        <v>2</v>
+      </c>
+      <c r="M5" s="2">
+        <v>1</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2">
+        <v>1</v>
+      </c>
+      <c r="P5" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>2</v>
+      </c>
+      <c r="R5" s="2">
+        <v>2</v>
+      </c>
+      <c r="S5" s="2">
+        <v>0</v>
+      </c>
+      <c r="T5" s="2">
+        <v>0</v>
+      </c>
+      <c r="U5" s="2">
+        <v>0</v>
+      </c>
+      <c r="V5" s="2">
+        <v>0</v>
+      </c>
+      <c r="W5" s="2">
+        <f>SUM(K5:V5)</f>
+        <v>10</v>
+      </c>
+      <c r="X5" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="Y5" s="11">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="Z5" s="12">
+        <f t="shared" si="2"/>
+        <v>0.7</v>
+      </c>
+      <c r="AA5" s="3">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A6" s="10">
+        <v>63991</v>
+      </c>
+      <c r="B6" s="1">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2</v>
+      </c>
+      <c r="G6" s="2">
+        <v>3</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2</v>
+      </c>
+      <c r="I6" s="2">
+        <v>2</v>
+      </c>
+      <c r="J6" s="2">
+        <f>SUM(D6:I6)</f>
+        <v>12</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1</v>
+      </c>
+      <c r="L6" s="2">
+        <v>2</v>
+      </c>
+      <c r="M6" s="2">
+        <v>1</v>
+      </c>
+      <c r="N6" s="2">
+        <v>2</v>
+      </c>
+      <c r="O6" s="2">
+        <v>1</v>
+      </c>
+      <c r="P6" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>3</v>
+      </c>
+      <c r="R6" s="2">
+        <v>2</v>
+      </c>
+      <c r="S6" s="2">
+        <v>3</v>
+      </c>
+      <c r="T6" s="2">
+        <v>5</v>
+      </c>
+      <c r="U6" s="2">
+        <v>1</v>
+      </c>
+      <c r="V6" s="2">
+        <v>2</v>
+      </c>
+      <c r="W6" s="2">
+        <f>SUM(K6:V6)</f>
+        <v>24</v>
+      </c>
+      <c r="X6" s="2">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="Y6" s="11">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="Z6" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AA6" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A7" s="10">
+        <v>79014</v>
+      </c>
+      <c r="B7" s="1">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2">
+        <f>SUM(D7:I7)</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2">
+        <f>SUM(K7:V7)</f>
+        <v>0</v>
+      </c>
+      <c r="X7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y7" s="11">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="Z7" s="12">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="AA7" s="3">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="K1:W1"/>
+    <mergeCell ref="X1:X2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>